<commit_message>
versão para ser testada
</commit_message>
<xml_diff>
--- a/examples/cloze/sc_or_s.xlsx
+++ b/examples/cloze/sc_or_s.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedrocruz\Documents\GitHub\pyequa\examples\cloze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9EB66F6-2E0C-4C3A-BE82-F2647FCB360A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD0B491-9538-41DE-BA05-FD23F68C08CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11235" xr2:uid="{025B3FE9-262F-4A56-9EA5-E26B9EB3C418}"/>
   </bookViews>
@@ -94,9 +94,6 @@
     <t>justificação</t>
   </si>
   <si>
-    <t>o desvio padrão corrigido é maior que o desvio padrão não corrigido</t>
-  </si>
-  <si>
     <t>o desvio padrão corrigido é aproximado ao desvio padrão não corrigido</t>
   </si>
   <si>
@@ -124,6 +121,9 @@
   </si>
   <si>
     <t>sympy</t>
+  </si>
+  <si>
+    <t>o desvio padrão corrigido é maior, ou bastante maior, que o desvio padrão não corrigido</t>
   </si>
 </sst>
 </file>
@@ -542,7 +542,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,10 +556,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>18</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>0</v>
@@ -587,7 +587,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -606,7 +606,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -625,7 +625,7 @@
         <v>1.1111111111111112</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -644,7 +644,7 @@
         <v>1.0526315789473684</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -663,7 +663,7 @@
         <v>1.0101010101010102</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -682,7 +682,7 @@
         <v>1.0010010010010011</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -720,7 +720,7 @@
     </row>
     <row r="2" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>3</v>
@@ -729,13 +729,13 @@
     </row>
     <row r="3" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="5"/>
     </row>
@@ -744,7 +744,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>13</v>
@@ -756,7 +756,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="5"/>
     </row>
@@ -765,7 +765,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="5"/>
     </row>
@@ -797,7 +797,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="225" customHeight="1" x14ac:dyDescent="0.25">
@@ -828,7 +828,7 @@
     </row>
     <row r="2" spans="1:1" ht="193.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
@@ -876,17 +876,17 @@
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
multichoice versão 0 parece funcionar
</commit_message>
<xml_diff>
--- a/examples/cloze/sc_or_s.xlsx
+++ b/examples/cloze/sc_or_s.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedrocruz\Documents\GitHub\pyequa\examples\cloze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD0B491-9538-41DE-BA05-FD23F68C08CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AF4F49-C7D3-408A-B666-04A6004082BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11235" xr2:uid="{025B3FE9-262F-4A56-9EA5-E26B9EB3C418}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{025B3FE9-262F-4A56-9EA5-E26B9EB3C418}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
@@ -40,15 +40,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>s_or_sc</t>
-  </si>
-  <si>
-    <t>deve ser usado o desvio padrão corrigido</t>
-  </si>
-  <si>
-    <t>pode ser usado o desvio padrão corrigido ou não</t>
   </si>
   <si>
     <t>racio_s_c_s</t>
@@ -94,9 +88,6 @@
     <t>justificação</t>
   </si>
   <si>
-    <t>o desvio padrão corrigido é aproximado ao desvio padrão não corrigido</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
@@ -123,7 +114,25 @@
     <t>sympy</t>
   </si>
   <si>
-    <t>o desvio padrão corrigido é maior, ou bastante maior, que o desvio padrão não corrigido</t>
+    <t>maior, ou bastante maior, que o</t>
+  </si>
+  <si>
+    <t>aproximado ao</t>
+  </si>
+  <si>
+    <t>corrigido</t>
+  </si>
+  <si>
+    <t>pode</t>
+  </si>
+  <si>
+    <t>deve</t>
+  </si>
+  <si>
+    <t>podedeve</t>
+  </si>
+  <si>
+    <t>corrigido ou não</t>
   </si>
 </sst>
 </file>
@@ -539,39 +548,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A89DB7D-2721-4F67-AD22-B28E1F1D30ED}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="50.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="72.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="72.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -580,17 +593,20 @@
         <v>'2'</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="9">
-        <f t="shared" ref="D2:D7" si="0">A2/(A2-1)</f>
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="9">
+        <f t="shared" ref="E2:E7" si="0">A2/(A2-1)</f>
         <v>2</v>
       </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -599,17 +615,20 @@
         <v>'4'</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="9">
         <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -618,17 +637,20 @@
         <v>'10'</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="9">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="9">
         <f t="shared" si="0"/>
         <v>1.1111111111111112</v>
       </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20</v>
       </c>
@@ -637,17 +659,20 @@
         <v>'20'</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="9">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="9">
         <f t="shared" si="0"/>
         <v>1.0526315789473684</v>
       </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>100</v>
       </c>
@@ -656,17 +681,20 @@
         <v>'100'</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="9">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="9">
         <f t="shared" si="0"/>
         <v>1.0101010101010102</v>
       </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1000</v>
       </c>
@@ -675,14 +703,17 @@
         <v>'1000'</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="9">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="9">
         <f t="shared" si="0"/>
         <v>1.0010010010010011</v>
       </c>
-      <c r="E7" t="s">
-        <v>15</v>
+      <c r="F7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -709,33 +740,33 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D3" s="5"/>
     </row>
@@ -744,28 +775,28 @@
         <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="D6" s="5"/>
     </row>
@@ -797,7 +828,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="225" customHeight="1" x14ac:dyDescent="0.25">
@@ -823,17 +854,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="193.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -841,12 +872,12 @@
     </row>
     <row r="5" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="195" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -866,27 +897,27 @@
   <sheetData>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>